<commit_message>
working top n recommendations
</commit_message>
<xml_diff>
--- a/data/test_database.xlsx
+++ b/data/test_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benwa\OneDrive\Desktop\side_projects\FlexLog\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a59d8b55efa33a7/Desktop/side_projects/FlexLog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0ACC65-8A63-4029-A50B-0BC675FD8894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{CB50CF43-697E-43DA-97A2-0404F61EC01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A85CDD17-0C8B-47F4-8B6C-7ADC51421FBE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5205" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{7F9B9716-D480-4CBE-A219-7F65C946ABFB}"/>
+    <workbookView xWindow="-28920" yWindow="5205" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7F9B9716-D480-4CBE-A219-7F65C946ABFB}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
   <si>
     <t>test</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>machine_type</t>
+  </si>
+  <si>
+    <t>isolation</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>first</t>
   </si>
 </sst>
 </file>
@@ -379,6 +388,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -729,11 +742,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B99E09-DC29-465C-9D48-23F81D030DB6}">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:S80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,9 +755,10 @@
     <col min="4" max="4" width="21.26953125" customWidth="1"/>
     <col min="11" max="11" width="13.453125" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="19" max="19" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -796,8 +810,14 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -813,8 +833,11 @@
       <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -833,8 +856,11 @@
       <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -853,8 +879,11 @@
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -870,8 +899,11 @@
       <c r="M5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -890,8 +922,11 @@
       <c r="M6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>A6+1</f>
         <v>6</v>
@@ -911,8 +946,11 @@
       <c r="M7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ref="A8:A71" si="0">A7+1</f>
         <v>7</v>
@@ -929,8 +967,11 @@
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -947,8 +988,11 @@
       <c r="P9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -968,8 +1012,11 @@
       <c r="P10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -989,8 +1036,11 @@
       <c r="P11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1007,8 +1057,11 @@
       <c r="M12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1025,8 +1078,11 @@
       <c r="O13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1046,8 +1102,11 @@
       <c r="O14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1064,8 +1123,11 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1079,8 +1141,11 @@
       <c r="N16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1094,8 +1159,11 @@
       <c r="Q17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1109,8 +1177,11 @@
       <c r="N18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1127,8 +1198,11 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1142,8 +1216,11 @@
       <c r="M20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1157,8 +1234,11 @@
       <c r="Q21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1172,8 +1252,11 @@
       <c r="O22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1187,8 +1270,11 @@
       <c r="Q23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1202,8 +1288,11 @@
       <c r="O24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1217,8 +1306,11 @@
       <c r="N25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1232,8 +1324,11 @@
       <c r="O26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1247,8 +1342,11 @@
       <c r="N27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1265,8 +1363,11 @@
       <c r="P28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1283,8 +1384,11 @@
       <c r="P29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1301,8 +1405,11 @@
       <c r="P30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1313,8 +1420,11 @@
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1325,8 +1435,11 @@
       <c r="G32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1337,8 +1450,11 @@
       <c r="G33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1349,8 +1465,11 @@
       <c r="G34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1361,8 +1480,11 @@
       <c r="G35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1373,8 +1495,11 @@
       <c r="G36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1385,8 +1510,11 @@
       <c r="G37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1397,8 +1525,11 @@
       <c r="G38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1409,8 +1540,11 @@
       <c r="K39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1421,8 +1555,11 @@
       <c r="K40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1436,8 +1573,11 @@
       <c r="K41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1451,8 +1591,11 @@
       <c r="K42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1466,8 +1609,11 @@
       <c r="G43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1481,8 +1627,11 @@
       <c r="G44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1496,8 +1645,11 @@
       <c r="G45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1508,8 +1660,11 @@
       <c r="G46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1526,8 +1681,11 @@
       <c r="M47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1544,8 +1702,11 @@
       <c r="P48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="S48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1565,8 +1726,11 @@
       <c r="O49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1586,8 +1750,11 @@
       <c r="O50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1607,8 +1774,11 @@
       <c r="M51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1628,8 +1798,11 @@
       <c r="M52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1646,8 +1819,11 @@
       <c r="N53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="S53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1667,8 +1843,11 @@
       <c r="L54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="S54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1688,8 +1867,11 @@
       <c r="L55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="S55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1706,8 +1888,11 @@
       <c r="N56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="S56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1724,8 +1909,11 @@
       <c r="M57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1745,8 +1933,11 @@
       <c r="M58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1763,8 +1954,11 @@
       <c r="M59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1784,8 +1978,11 @@
       <c r="M60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1802,8 +1999,11 @@
       <c r="M61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1823,8 +2023,11 @@
       <c r="O62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1844,8 +2047,11 @@
       <c r="O63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1862,8 +2068,11 @@
       <c r="L64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1883,8 +2092,11 @@
       <c r="O65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1901,8 +2113,11 @@
       <c r="N66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1919,8 +2134,11 @@
       <c r="N67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -1937,8 +2155,11 @@
       <c r="Q68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -1955,8 +2176,11 @@
       <c r="M69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -1973,8 +2197,11 @@
       <c r="M70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -1991,8 +2218,11 @@
       <c r="Q71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" ref="A72:A80" si="1">A71+1</f>
         <v>71</v>
@@ -2009,8 +2239,11 @@
       <c r="M72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -2027,8 +2260,11 @@
       <c r="Q73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -2048,8 +2284,11 @@
       <c r="O74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -2069,8 +2308,11 @@
       <c r="O75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -2090,8 +2332,11 @@
       <c r="O76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -2108,8 +2353,11 @@
       <c r="O77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -2126,8 +2374,11 @@
       <c r="O78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -2144,8 +2395,11 @@
       <c r="O79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -2160,6 +2414,9 @@
         <v>1</v>
       </c>
       <c r="N80">
+        <v>1</v>
+      </c>
+      <c r="R80">
         <v>1</v>
       </c>
     </row>
@@ -2170,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09938836-A522-4862-9EDC-802AAFC46EC8}">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2185,7 +2442,7 @@
     <col min="6" max="6" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2204,8 +2461,11 @@
       <c r="F1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2224,8 +2484,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2244,8 +2507,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2264,8 +2530,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2284,8 +2553,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2304,8 +2576,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2324,8 +2599,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2344,8 +2622,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2364,8 +2645,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2384,8 +2668,11 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2404,8 +2691,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2424,8 +2714,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2444,8 +2737,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2464,8 +2760,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2484,8 +2783,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2504,8 +2806,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2524,8 +2829,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2544,8 +2852,11 @@
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2564,8 +2875,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2584,8 +2898,11 @@
       <c r="F20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2604,8 +2921,11 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2624,8 +2944,11 @@
       <c r="F22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2644,8 +2967,11 @@
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2664,8 +2990,11 @@
       <c r="F24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2684,8 +3013,11 @@
       <c r="F25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2704,8 +3036,11 @@
       <c r="F26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2724,8 +3059,11 @@
       <c r="F27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2744,8 +3082,11 @@
       <c r="F28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2764,8 +3105,11 @@
       <c r="F29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2784,8 +3128,11 @@
       <c r="F30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2804,8 +3151,11 @@
       <c r="F31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2824,8 +3174,11 @@
       <c r="F32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2844,8 +3197,11 @@
       <c r="F33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2864,8 +3220,11 @@
       <c r="F34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2884,8 +3243,11 @@
       <c r="F35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2904,8 +3266,11 @@
       <c r="F36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2924,8 +3289,11 @@
       <c r="F37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2944,8 +3312,11 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2964,8 +3335,11 @@
       <c r="F39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2984,8 +3358,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3004,8 +3381,11 @@
       <c r="F41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3024,8 +3404,11 @@
       <c r="F42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3044,8 +3427,11 @@
       <c r="F43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3064,8 +3450,11 @@
       <c r="F44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3084,8 +3473,11 @@
       <c r="F45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3104,8 +3496,11 @@
       <c r="F46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3124,8 +3519,11 @@
       <c r="F47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3144,8 +3542,11 @@
       <c r="F48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3164,8 +3565,11 @@
       <c r="F49">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3184,8 +3588,11 @@
       <c r="F50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1</v>
       </c>
@@ -3204,8 +3611,11 @@
       <c r="F51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1</v>
       </c>
@@ -3224,8 +3634,11 @@
       <c r="F52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1</v>
       </c>
@@ -3244,8 +3657,11 @@
       <c r="F53">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3265,7 +3681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1</v>
       </c>
@@ -3285,7 +3701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1</v>
       </c>
@@ -3305,7 +3721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
@@ -3324,8 +3740,11 @@
       <c r="F57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1</v>
       </c>
@@ -3344,8 +3763,11 @@
       <c r="F58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
@@ -3365,7 +3787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1</v>
       </c>
@@ -3385,7 +3807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1</v>
       </c>
@@ -3405,7 +3827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1</v>
       </c>
@@ -3425,7 +3847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1</v>
       </c>
@@ -3445,7 +3867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1</v>
       </c>
@@ -3465,7 +3887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1</v>
       </c>
@@ -3485,7 +3907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1</v>
       </c>
@@ -3505,7 +3927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1</v>
       </c>
@@ -3525,7 +3947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1</v>
       </c>
@@ -3545,7 +3967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1</v>
       </c>
@@ -3565,7 +3987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1</v>
       </c>
@@ -3585,7 +4007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1</v>
       </c>
@@ -3605,7 +4027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1</v>
       </c>
@@ -3624,8 +4046,11 @@
       <c r="F72">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1</v>
       </c>
@@ -3644,8 +4069,11 @@
       <c r="F73">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1</v>
       </c>
@@ -3664,8 +4092,11 @@
       <c r="F74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
@@ -3685,7 +4116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1</v>
       </c>
@@ -3705,7 +4136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1</v>
       </c>
@@ -3725,7 +4156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1</v>
       </c>
@@ -3745,7 +4176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1</v>
       </c>
@@ -3765,7 +4196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1</v>
       </c>
@@ -3785,7 +4216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1</v>
       </c>
@@ -3805,7 +4236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1</v>
       </c>
@@ -3825,7 +4256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1</v>
       </c>
@@ -3845,7 +4276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1</v>
       </c>
@@ -3865,7 +4296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1</v>
       </c>
@@ -3885,7 +4316,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1</v>
       </c>
@@ -3905,7 +4336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1</v>
       </c>
@@ -3924,8 +4355,11 @@
       <c r="F87">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1</v>
       </c>
@@ -3944,8 +4378,11 @@
       <c r="F88">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1</v>
       </c>
@@ -3964,8 +4401,11 @@
       <c r="F89">
         <v>7</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1</v>
       </c>
@@ -3985,7 +4425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1</v>
       </c>
@@ -4005,7 +4445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1</v>
       </c>
@@ -4025,7 +4465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1</v>
       </c>
@@ -4045,7 +4485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1</v>
       </c>
@@ -4065,7 +4505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1</v>
       </c>
@@ -4085,7 +4525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1</v>
       </c>
@@ -4105,7 +4545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1</v>
       </c>
@@ -4125,7 +4565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1</v>
       </c>
@@ -4145,7 +4585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>1</v>
       </c>
@@ -4165,7 +4605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1</v>
       </c>
@@ -4185,7 +4625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1</v>
       </c>
@@ -4205,7 +4645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1</v>
       </c>
@@ -4224,8 +4664,11 @@
       <c r="F102">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>1</v>
       </c>
@@ -4244,8 +4687,11 @@
       <c r="F103">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1</v>
       </c>
@@ -4265,7 +4711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>1</v>
       </c>
@@ -4285,7 +4731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1</v>
       </c>
@@ -4305,7 +4751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1</v>
       </c>
@@ -4325,7 +4771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>1</v>
       </c>
@@ -4345,7 +4791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1</v>
       </c>
@@ -4365,7 +4811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>1</v>
       </c>
@@ -4394,8 +4840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14970B67-C41F-4516-BA66-F609F73B9329}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
altered schema, added feature manager, one-hot encoding function
</commit_message>
<xml_diff>
--- a/data/test_database.xlsx
+++ b/data/test_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a59d8b55efa33a7/Desktop/side_projects/FlexLog/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benwa\OneDrive\Desktop\side_projects\FlexLog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{CB50CF43-697E-43DA-97A2-0404F61EC01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A85CDD17-0C8B-47F4-8B6C-7ADC51421FBE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A128ECE-A7EA-4873-923F-760A7037D766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5205" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7F9B9716-D480-4CBE-A219-7F65C946ABFB}"/>
+    <workbookView xWindow="-28920" yWindow="5205" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F9B9716-D480-4CBE-A219-7F65C946ABFB}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="109">
   <si>
     <t>test</t>
   </si>
@@ -72,9 +72,6 @@
     <t>triceps</t>
   </si>
   <si>
-    <t>misc_group</t>
-  </si>
-  <si>
     <t>barbell</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>smith</t>
   </si>
   <si>
-    <t>misc_machine</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>bench press</t>
   </si>
   <si>
-    <t>high-to-low</t>
-  </si>
-  <si>
     <t>pec-dec fly</t>
   </si>
   <si>
@@ -174,18 +165,9 @@
     <t xml:space="preserve">calf raise </t>
   </si>
   <si>
-    <t>incline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decline </t>
-  </si>
-  <si>
     <t xml:space="preserve">bench press </t>
   </si>
   <si>
-    <t>low-to-high</t>
-  </si>
-  <si>
     <t xml:space="preserve">foot supported row </t>
   </si>
   <si>
@@ -201,15 +183,9 @@
     <t>smith machine</t>
   </si>
   <si>
-    <t xml:space="preserve">barbell </t>
-  </si>
-  <si>
     <t>seated</t>
   </si>
   <si>
-    <t xml:space="preserve">standing </t>
-  </si>
-  <si>
     <t>standing</t>
   </si>
   <si>
@@ -222,21 +198,12 @@
     <t>chest press</t>
   </si>
   <si>
-    <t xml:space="preserve">smith </t>
-  </si>
-  <si>
     <t xml:space="preserve">chest press </t>
   </si>
   <si>
     <t xml:space="preserve">chest fly </t>
   </si>
   <si>
-    <t xml:space="preserve">fly </t>
-  </si>
-  <si>
-    <t>fly</t>
-  </si>
-  <si>
     <t>shrug</t>
   </si>
   <si>
@@ -252,18 +219,9 @@
     <t>single-arm</t>
   </si>
   <si>
-    <t>double-arm</t>
-  </si>
-  <si>
     <t xml:space="preserve">overhead press </t>
   </si>
   <si>
-    <t xml:space="preserve">dumbbell </t>
-  </si>
-  <si>
-    <t>curl</t>
-  </si>
-  <si>
     <t>hammer curl</t>
   </si>
   <si>
@@ -334,6 +292,81 @@
   </si>
   <si>
     <t>first</t>
+  </si>
+  <si>
+    <t>incline barbell</t>
+  </si>
+  <si>
+    <t>decline barbell</t>
+  </si>
+  <si>
+    <t>incline dumbbell</t>
+  </si>
+  <si>
+    <t>decline dumbbell</t>
+  </si>
+  <si>
+    <t>incline smith</t>
+  </si>
+  <si>
+    <t>decline smith</t>
+  </si>
+  <si>
+    <t>chest fly</t>
+  </si>
+  <si>
+    <t>mid cable</t>
+  </si>
+  <si>
+    <t>low-to-high cable</t>
+  </si>
+  <si>
+    <t>high-to-low cable</t>
+  </si>
+  <si>
+    <t>single-arm cable</t>
+  </si>
+  <si>
+    <t>cross cable</t>
+  </si>
+  <si>
+    <t>standing dumbbell</t>
+  </si>
+  <si>
+    <t>seated dumbbell</t>
+  </si>
+  <si>
+    <t>standing barbell</t>
+  </si>
+  <si>
+    <t>seated barbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rope </t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>dumbbell curl</t>
+  </si>
+  <si>
+    <t>cable curl</t>
+  </si>
+  <si>
+    <t>barbell curl</t>
+  </si>
+  <si>
+    <t>machine curl</t>
+  </si>
+  <si>
+    <t>muscle_group</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>exercise_type</t>
   </si>
 </sst>
 </file>
@@ -388,10 +421,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -742,1682 +771,1625 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B99E09-DC29-465C-9D48-23F81D030DB6}">
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C77" sqref="C77"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
-    <col min="17" max="17" width="17" customWidth="1"/>
-    <col min="19" max="19" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
+    <col min="18" max="18" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>95</v>
-      </c>
-      <c r="S1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>A6+1</f>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ref="A8:A71" si="0">A7+1</f>
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
       <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
         <v>59</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <f t="shared" si="0"/>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
         <v>60</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <f t="shared" si="0"/>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <f t="shared" si="0"/>
+      <c r="E70" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="F70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71" t="s">
         <v>67</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="S28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="R29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="P30">
-        <v>1</v>
-      </c>
-      <c r="R30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="S31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="S32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="S33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="D34" t="s">
-        <v>37</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="S34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="S35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="S36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="D37" t="s">
-        <v>40</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="R37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="D38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="R38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="D39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="R39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="D40" t="s">
-        <v>42</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="R40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" t="s">
-        <v>43</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-      <c r="R41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" t="s">
-        <v>43</v>
-      </c>
-      <c r="K42">
-        <v>1</v>
-      </c>
-      <c r="R42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" t="s">
-        <v>40</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="R43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" t="s">
-        <v>51</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="R44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="R45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="D46" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="R46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" t="s">
-        <v>71</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-      <c r="M47">
-        <v>1</v>
-      </c>
-      <c r="S47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" t="s">
-        <v>71</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="P48">
-        <v>1</v>
-      </c>
-      <c r="S48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>69</v>
-      </c>
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" t="s">
-        <v>57</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="O49">
-        <v>1</v>
-      </c>
-      <c r="R49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" t="s">
-        <v>57</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="O50">
-        <v>1</v>
-      </c>
-      <c r="R50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" t="s">
-        <v>68</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="M51">
-        <v>1</v>
-      </c>
-      <c r="R51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" t="s">
-        <v>57</v>
-      </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="M52">
-        <v>1</v>
-      </c>
-      <c r="R52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" t="s">
-        <v>71</v>
-      </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="N53">
-        <v>1</v>
-      </c>
-      <c r="S53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s">
-        <v>71</v>
-      </c>
-      <c r="H54">
-        <v>1</v>
-      </c>
-      <c r="L54">
-        <v>1</v>
-      </c>
-      <c r="S54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" t="s">
-        <v>71</v>
-      </c>
-      <c r="H55">
-        <v>1</v>
-      </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-      <c r="S55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" t="s">
-        <v>71</v>
-      </c>
-      <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="N56">
-        <v>1</v>
-      </c>
-      <c r="S56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="C57" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" t="s">
-        <v>73</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="M57">
-        <v>1</v>
-      </c>
-      <c r="R57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-      <c r="M58">
-        <v>1</v>
-      </c>
-      <c r="R58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" t="s">
-        <v>74</v>
-      </c>
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="M59">
-        <v>1</v>
-      </c>
-      <c r="R59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D60" t="s">
-        <v>75</v>
-      </c>
-      <c r="I60">
-        <v>1</v>
-      </c>
-      <c r="M60">
-        <v>1</v>
-      </c>
-      <c r="R60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C61" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" t="s">
-        <v>76</v>
-      </c>
-      <c r="I61">
-        <v>1</v>
-      </c>
-      <c r="M61">
-        <v>1</v>
-      </c>
-      <c r="R61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>77</v>
-      </c>
-      <c r="C62" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" t="s">
-        <v>73</v>
-      </c>
-      <c r="I62">
-        <v>1</v>
-      </c>
-      <c r="O62">
-        <v>1</v>
-      </c>
-      <c r="R62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>78</v>
-      </c>
-      <c r="C63" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" t="s">
-        <v>73</v>
-      </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-      <c r="O63">
-        <v>1</v>
-      </c>
-      <c r="R63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="C64" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" t="s">
-        <v>73</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="L64">
-        <v>1</v>
-      </c>
-      <c r="R64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" t="s">
-        <v>73</v>
-      </c>
-      <c r="I65">
-        <v>1</v>
-      </c>
-      <c r="O65">
-        <v>1</v>
-      </c>
-      <c r="R65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C66" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" t="s">
-        <v>73</v>
-      </c>
-      <c r="I66">
-        <v>1</v>
-      </c>
-      <c r="N66">
-        <v>1</v>
-      </c>
-      <c r="R66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="C67" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" t="s">
-        <v>79</v>
-      </c>
-      <c r="I67">
-        <v>1</v>
-      </c>
-      <c r="N67">
-        <v>1</v>
-      </c>
-      <c r="R67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="C68" t="s">
-        <v>80</v>
-      </c>
-      <c r="D68" t="s">
-        <v>79</v>
-      </c>
-      <c r="I68">
-        <v>1</v>
-      </c>
-      <c r="Q68">
-        <v>1</v>
-      </c>
-      <c r="R68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="C69" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" t="s">
-        <v>79</v>
-      </c>
-      <c r="I69">
-        <v>1</v>
-      </c>
-      <c r="M69">
-        <v>1</v>
-      </c>
-      <c r="R69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="C70" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>107</v>
+      </c>
+      <c r="F71" t="s">
         <v>81</v>
       </c>
-      <c r="J70">
-        <v>1</v>
-      </c>
-      <c r="M70">
-        <v>1</v>
-      </c>
-      <c r="R70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>80</v>
-      </c>
-      <c r="D71" t="s">
-        <v>81</v>
-      </c>
-      <c r="J71">
-        <v>1</v>
-      </c>
-      <c r="Q71">
-        <v>1</v>
-      </c>
-      <c r="R71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" ref="A72:A80" si="1">A71+1</f>
         <v>71</v>
       </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
       <c r="C72" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D72" t="s">
-        <v>82</v>
-      </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-      <c r="M72">
-        <v>1</v>
-      </c>
-      <c r="R72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
+      <c r="B73" t="s">
+        <v>66</v>
+      </c>
       <c r="C73" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
-      </c>
-      <c r="J73">
-        <v>1</v>
-      </c>
-      <c r="Q73">
-        <v>1</v>
-      </c>
-      <c r="R73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D74" t="s">
-        <v>83</v>
-      </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
-      <c r="O74">
-        <v>1</v>
-      </c>
-      <c r="R74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E74" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="D75" t="s">
-        <v>82</v>
-      </c>
-      <c r="J75">
-        <v>1</v>
-      </c>
-      <c r="O75">
-        <v>1</v>
-      </c>
-      <c r="R75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="D76" t="s">
-        <v>82</v>
-      </c>
-      <c r="J76">
-        <v>1</v>
-      </c>
-      <c r="O76">
-        <v>1</v>
-      </c>
-      <c r="R76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="C77" t="s">
+        <v>72</v>
       </c>
       <c r="D77" t="s">
-        <v>86</v>
-      </c>
-      <c r="J77">
-        <v>1</v>
-      </c>
-      <c r="O77">
-        <v>1</v>
-      </c>
-      <c r="R77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>70</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
       </c>
       <c r="D78" t="s">
-        <v>86</v>
-      </c>
-      <c r="J78">
-        <v>1</v>
-      </c>
-      <c r="O78">
-        <v>1</v>
-      </c>
-      <c r="R78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
       </c>
       <c r="D79" t="s">
-        <v>86</v>
-      </c>
-      <c r="J79">
-        <v>1</v>
-      </c>
-      <c r="O79">
-        <v>1</v>
-      </c>
-      <c r="R79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="C80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s">
         <v>13</v>
       </c>
-      <c r="D80" t="s">
-        <v>86</v>
-      </c>
-      <c r="J80">
-        <v>1</v>
-      </c>
-      <c r="N80">
-        <v>1</v>
-      </c>
-      <c r="R80">
-        <v>1</v>
+      <c r="F80" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09938836-A522-4862-9EDC-802AAFC46EC8}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView topLeftCell="A78" workbookViewId="0">
       <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
@@ -2444,25 +2416,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -4857,10 +4829,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -4877,7 +4849,7 @@
         <v>46028</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -4891,7 +4863,7 @@
         <v>46030</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -4905,7 +4877,7 @@
         <v>46032</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -4919,7 +4891,7 @@
         <v>46033</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -4933,7 +4905,7 @@
         <v>46035</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -4947,7 +4919,7 @@
         <v>46037</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -4961,7 +4933,7 @@
         <v>46039</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -4975,7 +4947,7 @@
         <v>46040</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4998,10 +4970,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>